<commit_message>
Homa page isn't good yet
</commit_message>
<xml_diff>
--- a/src/main/resources/import-product-excel.xlsx
+++ b/src/main/resources/import-product-excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B256AC-E18E-4E72-B7AA-F34B4BC7119A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26CD4A2-F9DC-4A72-90D7-E254FF3AF68B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>product_name</t>
   </si>
@@ -32,6 +32,48 @@
   </si>
   <si>
     <t>Sanyo S23</t>
+  </si>
+  <si>
+    <t>product_pic</t>
+  </si>
+  <si>
+    <t>productPrice</t>
+  </si>
+  <si>
+    <t>/static/img/product-01.jpg</t>
+  </si>
+  <si>
+    <t>Sanyo S24</t>
+  </si>
+  <si>
+    <t>Sanyo S25</t>
+  </si>
+  <si>
+    <t>Sanyo S26</t>
+  </si>
+  <si>
+    <t>Sanyo S27</t>
+  </si>
+  <si>
+    <t>Sanyo S28</t>
+  </si>
+  <si>
+    <t>Sanyo S29</t>
+  </si>
+  <si>
+    <t>Sanyo S30</t>
+  </si>
+  <si>
+    <t>Sanyo S31</t>
+  </si>
+  <si>
+    <t>Sanyo S32</t>
+  </si>
+  <si>
+    <t>Sanyo S33</t>
+  </si>
+  <si>
+    <t>Sanyo S34</t>
   </si>
 </sst>
 </file>
@@ -349,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -360,20 +402,186 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>